<commit_message>
update nach Open Space/ Präsi für Audit3
</commit_message>
<xml_diff>
--- a/Artefakte/WS2122_ChouliarasBurgdorfWolf_PoC_V02.xlsx
+++ b/Artefakte/WS2122_ChouliarasBurgdorfWolf_PoC_V02.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Studium\Semester_5\EP\EPW2122ChouliarasBurgdorfWolf\Artefakte\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Entwicklungsprojekt\EPW2122ChouliarasBurgdorfWolf\Artefakte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D977115F-373F-4B3F-85CC-179116FD1400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA2043A-2E00-4C4D-991D-1765ED759157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="93">
   <si>
     <t>Success</t>
   </si>
@@ -323,10 +323,22 @@
     <t>Das Wechseln ist nicht möglich.</t>
   </si>
   <si>
-    <t>Das Wechseln nicht möglich.</t>
-  </si>
-  <si>
     <t>Verwendung von 2D-Karten anstelle der Orthografischen Vogelperspektive</t>
+  </si>
+  <si>
+    <t>Ein Abgewandelter A-Star Algorithmus wurde implementiert</t>
+  </si>
+  <si>
+    <t>Ausgabe der Objektinformationen aus Blender ist gelungen.</t>
+  </si>
+  <si>
+    <t>Ist im Prototypen mit Würfeln gelungen.</t>
+  </si>
+  <si>
+    <t>Das Wechseln ist möglich.</t>
+  </si>
+  <si>
+    <t>Kamera kann durch einen Button gewechselt werden.</t>
   </si>
 </sst>
 </file>
@@ -473,7 +485,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -522,16 +534,23 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1360,18 +1379,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D5EE435-9524-4D5A-BEB4-5EBAA1BB63EA}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="3" width="22.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" customWidth="1"/>
+    <col min="6" max="6" width="31.5703125" customWidth="1"/>
     <col min="8" max="8" width="58" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1394,129 +1415,227 @@
       <c r="J2" s="6"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>43</v>
-      </c>
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="18"/>
       <c r="K3" s="18"/>
       <c r="L3" s="18"/>
     </row>
-    <row r="4" spans="1:12" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="E4" s="9"/>
+    <row r="4" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>43</v>
+      </c>
       <c r="H4" s="19"/>
       <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-    </row>
-    <row r="5" spans="1:12" ht="141.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>73</v>
-      </c>
+    </row>
+    <row r="5" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="E5" s="9"/>
+        <v>70</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>88</v>
+      </c>
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-    </row>
-    <row r="6" spans="1:12" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>79</v>
-      </c>
+    </row>
+    <row r="6" spans="1:12" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="E6" s="9"/>
+        <v>80</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>90</v>
+      </c>
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-    </row>
-    <row r="7" spans="1:12" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>75</v>
-      </c>
+    </row>
+    <row r="7" spans="1:12" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="9" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="E7" s="9"/>
+        <v>82</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>90</v>
+      </c>
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-    </row>
-    <row r="8" spans="1:12" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>85</v>
-      </c>
+    </row>
+    <row r="8" spans="1:12" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="E8" s="9"/>
+        <v>76</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>89</v>
+      </c>
       <c r="H8" s="19"/>
       <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
+    </row>
+    <row r="9" spans="1:12" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D14" s="6"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D16" s="22"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D17" s="22"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D18" s="22"/>
+    </row>
+    <row r="19" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="63" x14ac:dyDescent="0.25">
+      <c r="B20" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" s="9"/>
+    </row>
+    <row r="21" spans="2:6" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="B21" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="F21" s="9"/>
+    </row>
+    <row r="22" spans="2:6" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F22" s="9"/>
+    </row>
+    <row r="23" spans="2:6" ht="63" x14ac:dyDescent="0.25">
+      <c r="B23" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F23" s="9"/>
+    </row>
+    <row r="24" spans="2:6" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="F24" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>